<commit_message>
correction and processed more subjects
</commit_message>
<xml_diff>
--- a/Tesis/Resultados/Escalon/CC/PIE_Izquierdo_layer_0.xlsx
+++ b/Tesis/Resultados/Escalon/CC/PIE_Izquierdo_layer_0.xlsx
@@ -31,76 +31,76 @@
     <t>W_o</t>
   </si>
   <si>
-    <t>[-0.16450496017932892]</t>
-  </si>
-  <si>
-    <t>[-0.31381955742836]</t>
-  </si>
-  <si>
-    <t>[0.5160955786705017]</t>
-  </si>
-  <si>
-    <t>[-0.24059666693210602]</t>
-  </si>
-  <si>
-    <t>[0.29261288046836853]</t>
-  </si>
-  <si>
-    <t>[0.6381415724754333]</t>
-  </si>
-  <si>
-    <t>[0.6857835650444031]</t>
-  </si>
-  <si>
-    <t>[0.19473116099834442]</t>
-  </si>
-  <si>
-    <t>[-0.6858114004135132]</t>
-  </si>
-  <si>
-    <t>[0.4698392450809479]</t>
-  </si>
-  <si>
-    <t>[0.3198961615562439]</t>
-  </si>
-  <si>
-    <t>[0.23121720552444458]</t>
-  </si>
-  <si>
-    <t>[-0.49100232124328613]</t>
-  </si>
-  <si>
-    <t>[-0.12925173342227936]</t>
-  </si>
-  <si>
-    <t>[0.5923032760620117]</t>
-  </si>
-  <si>
-    <t>[0.34064269065856934]</t>
-  </si>
-  <si>
-    <t>[-0.36921143531799316]</t>
-  </si>
-  <si>
-    <t>[-0.11177253723144531]</t>
-  </si>
-  <si>
-    <t>[0.5653767585754395]</t>
-  </si>
-  <si>
-    <t>[-0.5200042724609375]</t>
-  </si>
-  <si>
-    <t>[0.41107767820358276]</t>
-  </si>
-  <si>
-    <t>[-0.11753720045089722]</t>
-  </si>
-  <si>
-    <t>[-0.6436423063278198]</t>
-  </si>
-  <si>
-    <t>[-0.31161677837371826]</t>
+    <t>[0.4790175259113312]</t>
+  </si>
+  <si>
+    <t>[-0.014327202923595905]</t>
+  </si>
+  <si>
+    <t>[0.20517955720424652]</t>
+  </si>
+  <si>
+    <t>[-0.5186729431152344]</t>
+  </si>
+  <si>
+    <t>[-0.30613699555397034]</t>
+  </si>
+  <si>
+    <t>[0.5261990427970886]</t>
+  </si>
+  <si>
+    <t>[0.6201562285423279]</t>
+  </si>
+  <si>
+    <t>[-0.18747356534004211]</t>
+  </si>
+  <si>
+    <t>[-0.37404918670654297]</t>
+  </si>
+  <si>
+    <t>[0.26703304052352905]</t>
+  </si>
+  <si>
+    <t>[0.458885133266449]</t>
+  </si>
+  <si>
+    <t>[-0.49441665410995483]</t>
+  </si>
+  <si>
+    <t>[-0.22918356955051422]</t>
+  </si>
+  <si>
+    <t>[0.49454209208488464]</t>
+  </si>
+  <si>
+    <t>[0.5160143971443176]</t>
+  </si>
+  <si>
+    <t>[-0.2571236193180084]</t>
+  </si>
+  <si>
+    <t>[-0.420513778924942]</t>
+  </si>
+  <si>
+    <t>[-0.23123757541179657]</t>
+  </si>
+  <si>
+    <t>[-0.6188594698905945]</t>
+  </si>
+  <si>
+    <t>[0.20336169004440308]</t>
+  </si>
+  <si>
+    <t>[0.38224339485168457]</t>
+  </si>
+  <si>
+    <t>[0.19735164940357208]</t>
+  </si>
+  <si>
+    <t>[0.6717901229858398]</t>
+  </si>
+  <si>
+    <t>[0.3735264539718628]</t>
   </si>
   <si>
     <t>U_i</t>
@@ -115,436 +115,436 @@
     <t>U_o</t>
   </si>
   <si>
-    <t>[0.3066519796848297]</t>
-  </si>
-  <si>
-    <t>[0.19404347240924835]</t>
-  </si>
-  <si>
-    <t>[0.18361517786979675]</t>
-  </si>
-  <si>
-    <t>[0.07331615686416626]</t>
-  </si>
-  <si>
-    <t>[0.36434799432754517]</t>
-  </si>
-  <si>
-    <t>[0.12552690505981445]</t>
-  </si>
-  <si>
-    <t>[0.5863111019134521]</t>
-  </si>
-  <si>
-    <t>[0.38150766491889954]</t>
-  </si>
-  <si>
-    <t>[-0.12584972381591797]</t>
-  </si>
-  <si>
-    <t>[0.16218151152133942]</t>
-  </si>
-  <si>
-    <t>[0.11473339796066284]</t>
-  </si>
-  <si>
-    <t>[0.08201441168785095]</t>
-  </si>
-  <si>
-    <t>[-0.16961681842803955]</t>
-  </si>
-  <si>
-    <t>[0.4047500193119049]</t>
-  </si>
-  <si>
-    <t>[0.19120635092258453]</t>
-  </si>
-  <si>
-    <t>[-0.41913583874702454]</t>
-  </si>
-  <si>
-    <t>[-0.1771998405456543]</t>
-  </si>
-  <si>
-    <t>[0.06641270965337753]</t>
-  </si>
-  <si>
-    <t>[0.1495819240808487]</t>
-  </si>
-  <si>
-    <t>[0.3237093687057495]</t>
-  </si>
-  <si>
-    <t>[0.1434430629014969]</t>
-  </si>
-  <si>
-    <t>[-0.027375830337405205]</t>
-  </si>
-  <si>
-    <t>[-0.3078838884830475]</t>
-  </si>
-  <si>
-    <t>[-0.021582715213298798]</t>
-  </si>
-  <si>
-    <t>[0.06662490218877792]</t>
-  </si>
-  <si>
-    <t>[-0.3590391278266907]</t>
-  </si>
-  <si>
-    <t>[-0.016981476917862892]</t>
-  </si>
-  <si>
-    <t>[-0.2671658992767334]</t>
-  </si>
-  <si>
-    <t>[0.24990901350975037]</t>
-  </si>
-  <si>
-    <t>[0.4618850648403168]</t>
-  </si>
-  <si>
-    <t>[0.5210928916931152]</t>
-  </si>
-  <si>
-    <t>[-0.056783076375722885]</t>
-  </si>
-  <si>
-    <t>[-0.2941368818283081]</t>
-  </si>
-  <si>
-    <t>[0.13375961780548096]</t>
-  </si>
-  <si>
-    <t>[0.28802695870399475]</t>
-  </si>
-  <si>
-    <t>[0.13413701951503754]</t>
-  </si>
-  <si>
-    <t>[-0.36931920051574707]</t>
-  </si>
-  <si>
-    <t>[0.35733363032341003]</t>
-  </si>
-  <si>
-    <t>[0.2999304533004761]</t>
-  </si>
-  <si>
-    <t>[-0.0067037115804851055]</t>
-  </si>
-  <si>
-    <t>[-0.44571006298065186]</t>
-  </si>
-  <si>
-    <t>[0.13242937624454498]</t>
-  </si>
-  <si>
-    <t>[0.32579702138900757]</t>
-  </si>
-  <si>
-    <t>[-0.18212224543094635]</t>
-  </si>
-  <si>
-    <t>[0.6588431596755981]</t>
-  </si>
-  <si>
-    <t>[0.14024901390075684]</t>
-  </si>
-  <si>
-    <t>[-0.5549939274787903]</t>
-  </si>
-  <si>
-    <t>[0.05671319738030434]</t>
-  </si>
-  <si>
-    <t>[-0.1192450076341629]</t>
-  </si>
-  <si>
-    <t>[-0.32063862681388855]</t>
-  </si>
-  <si>
-    <t>[0.10923886299133301]</t>
-  </si>
-  <si>
-    <t>[0.47544997930526733]</t>
-  </si>
-  <si>
-    <t>[-0.6296012997627258]</t>
-  </si>
-  <si>
-    <t>[0.00981697253882885]</t>
-  </si>
-  <si>
-    <t>[-0.2130778282880783]</t>
-  </si>
-  <si>
-    <t>[0.0020974825602024794]</t>
-  </si>
-  <si>
-    <t>[0.3602401912212372]</t>
-  </si>
-  <si>
-    <t>[0.1260615885257721]</t>
-  </si>
-  <si>
-    <t>[-0.3446911573410034]</t>
-  </si>
-  <si>
-    <t>[0.11145006865262985]</t>
-  </si>
-  <si>
-    <t>[-0.1978028118610382]</t>
-  </si>
-  <si>
-    <t>[-0.22198285162448883]</t>
-  </si>
-  <si>
-    <t>[-0.27635854482650757]</t>
-  </si>
-  <si>
-    <t>[-0.06401033699512482]</t>
-  </si>
-  <si>
-    <t>[0.06109057739377022]</t>
-  </si>
-  <si>
-    <t>[-0.3349200189113617]</t>
-  </si>
-  <si>
-    <t>[-0.3915286660194397]</t>
-  </si>
-  <si>
-    <t>[0.23300498723983765]</t>
-  </si>
-  <si>
-    <t>[-0.12970538437366486]</t>
-  </si>
-  <si>
-    <t>[-0.1707702875137329]</t>
-  </si>
-  <si>
-    <t>[0.42951899766921997]</t>
-  </si>
-  <si>
-    <t>[-0.11153744161128998]</t>
-  </si>
-  <si>
-    <t>[0.18014967441558838]</t>
-  </si>
-  <si>
-    <t>[0.05135992541909218]</t>
-  </si>
-  <si>
-    <t>[-0.14445249736309052]</t>
-  </si>
-  <si>
-    <t>[-0.06732266396284103]</t>
-  </si>
-  <si>
-    <t>[-0.25687897205352783]</t>
-  </si>
-  <si>
-    <t>[-0.6305521726608276]</t>
-  </si>
-  <si>
-    <t>[-0.1446058750152588]</t>
-  </si>
-  <si>
-    <t>[-0.02088281698524952]</t>
-  </si>
-  <si>
-    <t>[0.34128281474113464]</t>
-  </si>
-  <si>
-    <t>[0.16463983058929443]</t>
-  </si>
-  <si>
-    <t>[-0.15327350795269012]</t>
-  </si>
-  <si>
-    <t>[-0.2221939116716385]</t>
-  </si>
-  <si>
-    <t>[-0.013641241006553173]</t>
-  </si>
-  <si>
-    <t>[-0.2553977370262146]</t>
-  </si>
-  <si>
-    <t>[-0.6405042409896851]</t>
-  </si>
-  <si>
-    <t>[0.09755926579236984]</t>
-  </si>
-  <si>
-    <t>[0.05096474662423134]</t>
-  </si>
-  <si>
-    <t>[-0.2132091075181961]</t>
-  </si>
-  <si>
-    <t>[0.1024884507060051]</t>
-  </si>
-  <si>
-    <t>[-0.032918255776166916]</t>
-  </si>
-  <si>
-    <t>[-0.0919310450553894]</t>
-  </si>
-  <si>
-    <t>[-0.5872379541397095]</t>
-  </si>
-  <si>
-    <t>[0.36357438564300537]</t>
-  </si>
-  <si>
-    <t>[-0.06391561776399612]</t>
-  </si>
-  <si>
-    <t>[-0.009878559038043022]</t>
-  </si>
-  <si>
-    <t>[0.12391620129346848]</t>
-  </si>
-  <si>
-    <t>[0.06049364060163498]</t>
-  </si>
-  <si>
-    <t>[-0.31568461656570435]</t>
-  </si>
-  <si>
-    <t>[0.11515194922685623]</t>
-  </si>
-  <si>
-    <t>[0.2875541150569916]</t>
-  </si>
-  <si>
-    <t>[0.4938640892505646]</t>
-  </si>
-  <si>
-    <t>[0.33125486969947815]</t>
-  </si>
-  <si>
-    <t>[-0.184431791305542]</t>
-  </si>
-  <si>
-    <t>[-0.29091906547546387]</t>
-  </si>
-  <si>
-    <t>[0.13616228103637695]</t>
-  </si>
-  <si>
-    <t>[-0.14102092385292053]</t>
-  </si>
-  <si>
-    <t>[-0.16798467934131622]</t>
-  </si>
-  <si>
-    <t>[-0.23632293939590454]</t>
-  </si>
-  <si>
-    <t>[0.2133491188287735]</t>
-  </si>
-  <si>
-    <t>[0.0544758103787899]</t>
-  </si>
-  <si>
-    <t>[-0.3761097192764282]</t>
-  </si>
-  <si>
-    <t>[0.40906593203544617]</t>
-  </si>
-  <si>
-    <t>[-0.034255899488925934]</t>
-  </si>
-  <si>
-    <t>[0.04778716340661049]</t>
-  </si>
-  <si>
-    <t>[0.600384533405304]</t>
-  </si>
-  <si>
-    <t>[0.1602087914943695]</t>
-  </si>
-  <si>
-    <t>[0.10994863510131836]</t>
-  </si>
-  <si>
-    <t>[0.16820402443408966]</t>
-  </si>
-  <si>
-    <t>[0.14421772956848145]</t>
-  </si>
-  <si>
-    <t>[0.2765941321849823]</t>
-  </si>
-  <si>
-    <t>[0.40427878499031067]</t>
-  </si>
-  <si>
-    <t>[-0.0002931395429186523]</t>
-  </si>
-  <si>
-    <t>[0.321694552898407]</t>
-  </si>
-  <si>
-    <t>[0.40270259976387024]</t>
-  </si>
-  <si>
-    <t>[0.09144266694784164]</t>
-  </si>
-  <si>
-    <t>[0.12697792053222656]</t>
-  </si>
-  <si>
-    <t>[-0.1013534665107727]</t>
-  </si>
-  <si>
-    <t>[-0.056644149124622345]</t>
-  </si>
-  <si>
-    <t>[-0.3044450581073761]</t>
-  </si>
-  <si>
-    <t>[0.21612277626991272]</t>
-  </si>
-  <si>
-    <t>[-0.19625328481197357]</t>
-  </si>
-  <si>
-    <t>[0.3829100728034973]</t>
-  </si>
-  <si>
-    <t>[0.08353069424629211]</t>
-  </si>
-  <si>
-    <t>[0.1237117201089859]</t>
-  </si>
-  <si>
-    <t>[-0.5843033194541931]</t>
-  </si>
-  <si>
-    <t>[0.3581249713897705]</t>
-  </si>
-  <si>
-    <t>[0.57076096534729]</t>
-  </si>
-  <si>
-    <t>[-0.3098945915699005]</t>
-  </si>
-  <si>
-    <t>[0.35998180508613586]</t>
-  </si>
-  <si>
-    <t>[0.39041996002197266]</t>
-  </si>
-  <si>
-    <t>[-0.27682098746299744]</t>
-  </si>
-  <si>
-    <t>[-0.09980480372905731]</t>
+    <t>[-0.11007698625326157]</t>
+  </si>
+  <si>
+    <t>[0.26522189378738403]</t>
+  </si>
+  <si>
+    <t>[-0.37114256620407104]</t>
+  </si>
+  <si>
+    <t>[0.24828341603279114]</t>
+  </si>
+  <si>
+    <t>[-0.007561259437352419]</t>
+  </si>
+  <si>
+    <t>[-0.014334290288388729]</t>
+  </si>
+  <si>
+    <t>[0.048988740891218185]</t>
+  </si>
+  <si>
+    <t>[0.17938023805618286]</t>
+  </si>
+  <si>
+    <t>[0.4082971513271332]</t>
+  </si>
+  <si>
+    <t>[-0.10182424634695053]</t>
+  </si>
+  <si>
+    <t>[0.042019668966531754]</t>
+  </si>
+  <si>
+    <t>[0.3720601201057434]</t>
+  </si>
+  <si>
+    <t>[0.14599654078483582]</t>
+  </si>
+  <si>
+    <t>[0.2542678415775299]</t>
+  </si>
+  <si>
+    <t>[0.029663756489753723]</t>
+  </si>
+  <si>
+    <t>[0.13251927495002747]</t>
+  </si>
+  <si>
+    <t>[0.1845330446958542]</t>
+  </si>
+  <si>
+    <t>[-0.5557051301002502]</t>
+  </si>
+  <si>
+    <t>[0.13306082785129547]</t>
+  </si>
+  <si>
+    <t>[-0.22639480233192444]</t>
+  </si>
+  <si>
+    <t>[-0.5757596492767334]</t>
+  </si>
+  <si>
+    <t>[0.001289061619900167]</t>
+  </si>
+  <si>
+    <t>[-0.22340725362300873]</t>
+  </si>
+  <si>
+    <t>[-0.4177743196487427]</t>
+  </si>
+  <si>
+    <t>[0.002302418230101466]</t>
+  </si>
+  <si>
+    <t>[-0.07523500174283981]</t>
+  </si>
+  <si>
+    <t>[0.021706318482756615]</t>
+  </si>
+  <si>
+    <t>[-0.11169934272766113]</t>
+  </si>
+  <si>
+    <t>[-0.05722628906369209]</t>
+  </si>
+  <si>
+    <t>[0.028987016528844833]</t>
+  </si>
+  <si>
+    <t>[0.08484610170125961]</t>
+  </si>
+  <si>
+    <t>[-0.1631649285554886]</t>
+  </si>
+  <si>
+    <t>[-0.4901377260684967]</t>
+  </si>
+  <si>
+    <t>[0.16726219654083252]</t>
+  </si>
+  <si>
+    <t>[-0.19664278626441956]</t>
+  </si>
+  <si>
+    <t>[0.09795983880758286]</t>
+  </si>
+  <si>
+    <t>[0.1589871495962143]</t>
+  </si>
+  <si>
+    <t>[-0.07178657501935959]</t>
+  </si>
+  <si>
+    <t>[0.29674065113067627]</t>
+  </si>
+  <si>
+    <t>[-0.30330392718315125]</t>
+  </si>
+  <si>
+    <t>[-0.5927800536155701]</t>
+  </si>
+  <si>
+    <t>[-0.08712521940469742]</t>
+  </si>
+  <si>
+    <t>[-0.08485846221446991]</t>
+  </si>
+  <si>
+    <t>[0.5931736826896667]</t>
+  </si>
+  <si>
+    <t>[0.27076563239097595]</t>
+  </si>
+  <si>
+    <t>[0.10425765812397003]</t>
+  </si>
+  <si>
+    <t>[0.5484262108802795]</t>
+  </si>
+  <si>
+    <t>[-0.2236330360174179]</t>
+  </si>
+  <si>
+    <t>[0.038039159029722214]</t>
+  </si>
+  <si>
+    <t>[0.14456096291542053]</t>
+  </si>
+  <si>
+    <t>[-0.01716684363782406]</t>
+  </si>
+  <si>
+    <t>[0.018179919570684433]</t>
+  </si>
+  <si>
+    <t>[0.04799552634358406]</t>
+  </si>
+  <si>
+    <t>[0.23749418556690216]</t>
+  </si>
+  <si>
+    <t>[-0.26989731192588806]</t>
+  </si>
+  <si>
+    <t>[0.026618050411343575]</t>
+  </si>
+  <si>
+    <t>[-0.5338010191917419]</t>
+  </si>
+  <si>
+    <t>[0.32789039611816406]</t>
+  </si>
+  <si>
+    <t>[0.04774528741836548]</t>
+  </si>
+  <si>
+    <t>[-0.1312423050403595]</t>
+  </si>
+  <si>
+    <t>[-0.3548610508441925]</t>
+  </si>
+  <si>
+    <t>[0.0205962136387825]</t>
+  </si>
+  <si>
+    <t>[0.25811514258384705]</t>
+  </si>
+  <si>
+    <t>[-0.26166272163391113]</t>
+  </si>
+  <si>
+    <t>[-0.03564026206731796]</t>
+  </si>
+  <si>
+    <t>[-0.336428701877594]</t>
+  </si>
+  <si>
+    <t>[-0.11891134828329086]</t>
+  </si>
+  <si>
+    <t>[-0.0328708179295063]</t>
+  </si>
+  <si>
+    <t>[0.23941397666931152]</t>
+  </si>
+  <si>
+    <t>[0.1951303780078888]</t>
+  </si>
+  <si>
+    <t>[0.2350139021873474]</t>
+  </si>
+  <si>
+    <t>[0.4743146002292633]</t>
+  </si>
+  <si>
+    <t>[-0.031830765306949615]</t>
+  </si>
+  <si>
+    <t>[0.352872759103775]</t>
+  </si>
+  <si>
+    <t>[0.4436625838279724]</t>
+  </si>
+  <si>
+    <t>[0.17808961868286133]</t>
+  </si>
+  <si>
+    <t>[-0.2956162989139557]</t>
+  </si>
+  <si>
+    <t>[0.3466815948486328]</t>
+  </si>
+  <si>
+    <t>[0.3169711232185364]</t>
+  </si>
+  <si>
+    <t>[-0.12013861536979675]</t>
+  </si>
+  <si>
+    <t>[-0.4393238425254822]</t>
+  </si>
+  <si>
+    <t>[0.29107049107551575]</t>
+  </si>
+  <si>
+    <t>[-0.08090448379516602]</t>
+  </si>
+  <si>
+    <t>[-0.2561505138874054]</t>
+  </si>
+  <si>
+    <t>[0.1804896593093872]</t>
+  </si>
+  <si>
+    <t>[0.14859183132648468]</t>
+  </si>
+  <si>
+    <t>[-0.053681157529354095]</t>
+  </si>
+  <si>
+    <t>[-0.03506631404161453]</t>
+  </si>
+  <si>
+    <t>[-0.2525387704372406]</t>
+  </si>
+  <si>
+    <t>[0.006469057872891426]</t>
+  </si>
+  <si>
+    <t>[-0.34744495153427124]</t>
+  </si>
+  <si>
+    <t>[0.4732743203639984]</t>
+  </si>
+  <si>
+    <t>[0.19626645743846893]</t>
+  </si>
+  <si>
+    <t>[0.22448936104774475]</t>
+  </si>
+  <si>
+    <t>[-0.1426648050546646]</t>
+  </si>
+  <si>
+    <t>[0.2389877736568451]</t>
+  </si>
+  <si>
+    <t>[0.24796344339847565]</t>
+  </si>
+  <si>
+    <t>[0.1742614060640335]</t>
+  </si>
+  <si>
+    <t>[-0.07247792184352875]</t>
+  </si>
+  <si>
+    <t>[-0.34673938155174255]</t>
+  </si>
+  <si>
+    <t>[0.048702772706747055]</t>
+  </si>
+  <si>
+    <t>[0.13367097079753876]</t>
+  </si>
+  <si>
+    <t>[0.2827143669128418]</t>
+  </si>
+  <si>
+    <t>[-0.08643145114183426]</t>
+  </si>
+  <si>
+    <t>[-0.6211859583854675]</t>
+  </si>
+  <si>
+    <t>[0.13807573914527893]</t>
+  </si>
+  <si>
+    <t>[0.004140366800129414]</t>
+  </si>
+  <si>
+    <t>[0.3615567982196808]</t>
+  </si>
+  <si>
+    <t>[-0.1034189909696579]</t>
+  </si>
+  <si>
+    <t>[-0.19746644794940948]</t>
+  </si>
+  <si>
+    <t>[0.33636510372161865]</t>
+  </si>
+  <si>
+    <t>[0.03419554606080055]</t>
+  </si>
+  <si>
+    <t>[-0.09999280422925949]</t>
+  </si>
+  <si>
+    <t>[0.20507335662841797]</t>
+  </si>
+  <si>
+    <t>[-0.3690166175365448]</t>
+  </si>
+  <si>
+    <t>[0.06855786591768265]</t>
+  </si>
+  <si>
+    <t>[0.3726801574230194]</t>
+  </si>
+  <si>
+    <t>[0.3733590543270111]</t>
+  </si>
+  <si>
+    <t>[-0.19983218610286713]</t>
+  </si>
+  <si>
+    <t>[0.0625290498137474]</t>
+  </si>
+  <si>
+    <t>[0.0422305203974247]</t>
+  </si>
+  <si>
+    <t>[0.16072452068328857]</t>
+  </si>
+  <si>
+    <t>[0.06342268735170364]</t>
+  </si>
+  <si>
+    <t>[0.4121846854686737]</t>
+  </si>
+  <si>
+    <t>[0.020160723477602005]</t>
+  </si>
+  <si>
+    <t>[-0.3418613076210022]</t>
+  </si>
+  <si>
+    <t>[0.1550108939409256]</t>
+  </si>
+  <si>
+    <t>[-0.012582603842020035]</t>
+  </si>
+  <si>
+    <t>[-0.5979917645454407]</t>
+  </si>
+  <si>
+    <t>[0.09612375497817993]</t>
+  </si>
+  <si>
+    <t>[-0.38939496874809265]</t>
+  </si>
+  <si>
+    <t>[0.09402257949113846]</t>
+  </si>
+  <si>
+    <t>[-0.39521902799606323]</t>
+  </si>
+  <si>
+    <t>[0.22233946621418]</t>
+  </si>
+  <si>
+    <t>[0.19106489419937134]</t>
+  </si>
+  <si>
+    <t>[0.021203579381108284]</t>
+  </si>
+  <si>
+    <t>[-0.07709134370088577]</t>
+  </si>
+  <si>
+    <t>[0.40444648265838623]</t>
+  </si>
+  <si>
+    <t>[-0.21528543531894684]</t>
+  </si>
+  <si>
+    <t>[0.5441012978553772]</t>
+  </si>
+  <si>
+    <t>[0.401205450296402]</t>
+  </si>
+  <si>
+    <t>[0.09650546312332153]</t>
+  </si>
+  <si>
+    <t>[0.09475436061620712]</t>
+  </si>
+  <si>
+    <t>[0.10357120633125305]</t>
   </si>
   <si>
     <t>b_i</t>
@@ -559,76 +559,76 @@
     <t>b_o</t>
   </si>
   <si>
-    <t>[-0.14220936596393585]</t>
-  </si>
-  <si>
-    <t>[1.1497339010238647]</t>
-  </si>
-  <si>
-    <t>[0.18286184966564178]</t>
-  </si>
-  <si>
-    <t>[-0.19665022194385529]</t>
-  </si>
-  <si>
-    <t>[0.2458162158727646]</t>
-  </si>
-  <si>
-    <t>[1.2351051568984985]</t>
-  </si>
-  <si>
-    <t>[0.2546083331108093]</t>
-  </si>
-  <si>
-    <t>[0.05815316364169121]</t>
-  </si>
-  <si>
-    <t>[-0.1770545244216919]</t>
-  </si>
-  <si>
-    <t>[1.0951380729675293]</t>
-  </si>
-  <si>
-    <t>[0.19859060645103455]</t>
-  </si>
-  <si>
-    <t>[0.005120080895721912]</t>
-  </si>
-  <si>
-    <t>[-0.2221444845199585]</t>
-  </si>
-  <si>
-    <t>[1.1900449991226196]</t>
-  </si>
-  <si>
-    <t>[0.23452387750148773]</t>
-  </si>
-  <si>
-    <t>[0.02642439492046833]</t>
-  </si>
-  <si>
-    <t>[-0.24706138670444489]</t>
-  </si>
-  <si>
-    <t>[1.1964167356491089]</t>
-  </si>
-  <si>
-    <t>[0.23290418088436127]</t>
-  </si>
-  <si>
-    <t>[0.03597871586680412]</t>
-  </si>
-  <si>
-    <t>[0.2693461775779724]</t>
-  </si>
-  <si>
-    <t>[1.2387419939041138]</t>
-  </si>
-  <si>
-    <t>[-0.265575110912323]</t>
-  </si>
-  <si>
-    <t>[-0.015084169805049896]</t>
+    <t>[0.1543692946434021]</t>
+  </si>
+  <si>
+    <t>[1.108141303062439]</t>
+  </si>
+  <si>
+    <t>[0.17883551120758057]</t>
+  </si>
+  <si>
+    <t>[0.0025806331541389227]</t>
+  </si>
+  <si>
+    <t>[-0.15201164782047272]</t>
+  </si>
+  <si>
+    <t>[1.0557844638824463]</t>
+  </si>
+  <si>
+    <t>[0.18061989545822144]</t>
+  </si>
+  <si>
+    <t>[-0.03770367428660393]</t>
+  </si>
+  <si>
+    <t>[-0.3658266067504883]</t>
+  </si>
+  <si>
+    <t>[1.1944522857666016]</t>
+  </si>
+  <si>
+    <t>[0.18015111982822418]</t>
+  </si>
+  <si>
+    <t>[-0.14719539880752563]</t>
+  </si>
+  <si>
+    <t>[-0.2165326476097107]</t>
+  </si>
+  <si>
+    <t>[1.1495411396026611]</t>
+  </si>
+  <si>
+    <t>[0.22492381930351257]</t>
+  </si>
+  <si>
+    <t>[-0.1805049479007721]</t>
+  </si>
+  <si>
+    <t>[-0.21064268052577972]</t>
+  </si>
+  <si>
+    <t>[1.2058320045471191]</t>
+  </si>
+  <si>
+    <t>[-0.2132127583026886]</t>
+  </si>
+  <si>
+    <t>[0.23789440095424652]</t>
+  </si>
+  <si>
+    <t>[0.25144660472869873]</t>
+  </si>
+  <si>
+    <t>[1.1977962255477905]</t>
+  </si>
+  <si>
+    <t>[0.23459571599960327]</t>
+  </si>
+  <si>
+    <t>[0.0734112560749054]</t>
   </si>
 </sst>
 </file>

</xml_diff>